<commit_message>
! Bugfix: take into account header and total row presence or absence * Refactoring: extracted methods from AsEnumerable for readability and for better support of upcoming features + Extra xml comments added * License updated in files to avoid spammers :(
</commit_message>
<xml_diff>
--- a/EPPlus.TableAsEnumerable.Tests/Resources/testsheets.xlsx
+++ b/EPPlus.TableAsEnumerable.Tests/Resources/testsheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +75,36 @@
     <t>Toyota</t>
   </si>
   <si>
+    <t>ACX-224</t>
+  </si>
+  <si>
+    <t>EU-225541</t>
+  </si>
+  <si>
+    <t>ABD-002</t>
+  </si>
+  <si>
+    <t>A-000123</t>
+  </si>
+  <si>
+    <t>FORD</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Orance</t>
+  </si>
+  <si>
     <t>License plate</t>
   </si>
   <si>
@@ -90,34 +120,7 @@
     <t>Is ready for traffic?</t>
   </si>
   <si>
-    <t>ACX-224</t>
-  </si>
-  <si>
-    <t>EU-225541</t>
-  </si>
-  <si>
-    <t>ABD-002</t>
-  </si>
-  <si>
-    <t>A-000123</t>
-  </si>
-  <si>
-    <t>FORD</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Gray</t>
-  </si>
-  <si>
-    <t>Orance</t>
+    <t>Összeg</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0\ [$USD]"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ [$USD]"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -160,14 +163,14 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0\ [$USD]"/>
+      <numFmt numFmtId="164" formatCode="#,##0\ [$USD]"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -205,15 +208,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TEST3" displayName="TEST3" ref="A1:F6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TEST3" displayName="TEST3" ref="A1:F7" totalsRowCount="1">
   <autoFilter ref="A1:F6"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="License plate"/>
+    <tableColumn id="1" name="License plate" totalsRowLabel="Összeg"/>
     <tableColumn id="2" name="Manufacturer"/>
-    <tableColumn id="3" name="Manufacturing date"/>
-    <tableColumn id="4" name="Price"/>
+    <tableColumn id="3" name="Manufacturing date" totalsRowFunction="max"/>
+    <tableColumn id="4" name="Price" totalsRowFunction="max"/>
     <tableColumn id="5" name="Color"/>
-    <tableColumn id="6" name="Is ready for traffic?"/>
+    <tableColumn id="6" name="Is ready for traffic?" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -698,10 +701,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,27 +718,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -747,7 +750,7 @@
         <v>3500</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -755,10 +758,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>40389</v>
@@ -767,7 +770,7 @@
         <v>4800</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -775,7 +778,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -787,7 +790,7 @@
         <v>12000</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -804,7 +807,7 @@
         <v>500</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -812,7 +815,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -821,10 +824,27 @@
         <v>1200</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1">
+        <f>SUBTOTAL(104,TEST3[Manufacturing date])</f>
+        <v>42073</v>
+      </c>
+      <c r="D7">
+        <f>SUBTOTAL(104,TEST3[Price])</f>
+        <v>12000</v>
+      </c>
+      <c r="F7">
+        <f>SUBTOTAL(103,TEST3[Is ready for traffic?])</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
! Improved nullable/null handling + Added Validate<> method + tests + ExcelTableConvertExceptionArgs now holds exact cell address + Prepared for release 1.1
</commit_message>
<xml_diff>
--- a/EPPlus.TableAsEnumerable.Tests/Resources/testsheets.xlsx
+++ b/EPPlus.TableAsEnumerable.Tests/Resources/testsheets.xlsx
@@ -208,8 +208,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TEST3" displayName="TEST3" ref="A1:F7" totalsRowCount="1">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TEST3" displayName="TEST3" ref="B2:G8" totalsRowCount="1">
+  <autoFilter ref="B2:G7"/>
   <tableColumns count="6">
     <tableColumn id="1" name="License plate" totalsRowLabel="Összeg"/>
     <tableColumn id="2" name="Manufacturer"/>
@@ -701,148 +701,148 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="1">
         <v>37245</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>3500</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="b">
+      <c r="G3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>40389</v>
       </c>
-      <c r="D3">
+      <c r="E4">
         <v>4800</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="b">
+      <c r="G4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D5" s="1">
         <v>42073</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>12000</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="b">
+      <c r="G5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D6" s="1">
         <v>33030</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>500</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="b">
+      <c r="G6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>1200</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="b">
+      <c r="G7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D8" s="1">
         <f>SUBTOTAL(104,TEST3[Manufacturing date])</f>
         <v>42073</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <f>SUBTOTAL(104,TEST3[Price])</f>
         <v>12000</v>
       </c>
-      <c r="F7">
+      <c r="G8">
         <f>SUBTOTAL(103,TEST3[Is ready for traffic?])</f>
         <v>5</v>
       </c>

</xml_diff>